<commit_message>
updated gerbers and BOMs
</commit_message>
<xml_diff>
--- a/HVPCB/HVPCB_BOM.xlsx
+++ b/HVPCB/HVPCB_BOM.xlsx
@@ -1,17 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertkirk/DocsLocal/UT/LHRE/cy_23/HVPCB/git/HVPCB_2023/HVPCB/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{244374A3-3089-D044-BCDB-B2042D09E117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="21580" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - HVPCB BOM" sheetId="1" r:id="rId4"/>
+    <sheet name="HVPCB_BOM" sheetId="3" r:id="rId1"/>
+    <sheet name="HVPCB_BOM_MOUSER" sheetId="1" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="126">
   <si>
     <t>HVPCB BOM</t>
   </si>
@@ -66,10 +89,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>CL10A106MQ8NNNC</t>
     </r>
@@ -86,10 +110,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>C1691</t>
     </r>
@@ -103,10 +128,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>CL10A225KO8NNNC</t>
     </r>
@@ -114,10 +140,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>C23630</t>
     </r>
@@ -131,10 +158,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>CL10B104KB8NNNC</t>
     </r>
@@ -142,10 +170,11 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>C1591</t>
     </r>
@@ -431,18 +460,23 @@
   </si>
   <si>
     <t>CONN-TH_43045-0200</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>HVPCB BOM (MOUSER)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="&quot;$&quot;0.000"/>
-    <numFmt numFmtId="60" formatCode="&quot;$&quot;0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -452,28 +486,39 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="13"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="14"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -611,69 +656,72 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="21">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -684,28 +732,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ff222222"/>
-      <rgbColor rgb="ff333333"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="FF222222"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -904,7 +1009,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -923,7 +1028,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +1058,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +1084,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +1110,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1136,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,7 +1162,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,7 +1188,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1109,7 +1214,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,7 +1240,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,7 +1266,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1174,9 +1279,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -1193,7 +1304,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1212,7 +1323,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,7 +1349,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1264,7 +1375,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1290,7 +1401,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1316,7 +1427,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1342,7 +1453,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1368,7 +1479,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1394,7 +1505,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1420,7 +1531,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1446,7 +1557,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,9 +1570,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1475,7 +1592,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1494,7 +1611,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1524,7 +1641,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1550,7 +1667,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1576,7 +1693,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1602,7 +1719,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1628,7 +1745,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1654,7 +1771,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1680,7 +1797,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1706,7 +1823,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1732,7 +1849,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1745,948 +1862,1110 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{165082D4-FDDC-324D-89BC-8A565DEA40B3}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:M23"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="3.35156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.26562" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
     <col min="3" max="4" width="16.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.17188" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.2266" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.07812" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.4062" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.2266" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.57812" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7266" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.35156" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s" s="3">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s" s="3">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s" s="3">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s" s="3">
+      <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s" s="3">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" t="s" s="3">
+      <c r="J2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K2" t="s" s="3">
+      <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s" s="3">
+      <c r="L2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M2" t="s" s="3">
+      <c r="M2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" t="s" s="6">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s" s="6">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s" s="6">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>2</v>
       </c>
-      <c r="G3" t="s" s="6">
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" t="s" s="6">
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" t="s" s="6">
+      <c r="I3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s" s="6">
+      <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s" s="6">
+      <c r="K3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="8">
-        <v>0.005</v>
-      </c>
-      <c r="M3" s="9">
-        <f>ROUNDUP(L3*F3,2)</f>
+      <c r="L3" s="7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" ref="M3:M23" si="0">ROUNDUP(L3*F3,2)</f>
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="10">
+    <row r="4" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" t="s" s="12">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s" s="12">
+      <c r="D4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s" s="12">
+      <c r="E4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>1</v>
       </c>
-      <c r="G4" t="s" s="12">
+      <c r="G4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H4" t="s" s="12">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" t="s" s="12">
+      <c r="I4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s" s="12">
+      <c r="J4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s" s="12">
+      <c r="K4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="14">
-        <v>0.005</v>
-      </c>
-      <c r="M4" s="15">
-        <f>ROUNDUP(L4*F4,2)</f>
+      <c r="L4" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="10">
+    <row r="5" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" t="s" s="12">
+      <c r="B5" s="10"/>
+      <c r="C5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s" s="12">
+      <c r="D5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s" s="12">
+      <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>2</v>
       </c>
-      <c r="G5" t="s" s="12">
+      <c r="G5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="H5" t="s" s="12">
+      <c r="H5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I5" t="s" s="12">
+      <c r="I5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s" s="12">
+      <c r="J5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s" s="12">
+      <c r="K5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="14">
-        <v>0.002</v>
-      </c>
-      <c r="M5" s="15">
-        <f>ROUNDUP(L5*F5,2)</f>
+      <c r="L5" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="10">
+    <row r="6" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" t="s" s="12">
+      <c r="B6" s="10"/>
+      <c r="C6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s" s="12">
+      <c r="D6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E6" t="s" s="12">
+      <c r="E6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>1</v>
       </c>
-      <c r="G6" t="s" s="12">
+      <c r="G6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H6" t="s" s="12">
+      <c r="H6" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I6" t="s" s="12">
+      <c r="I6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J6" t="s" s="12">
+      <c r="J6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K6" t="s" s="12">
+      <c r="K6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M6" s="15">
-        <f>ROUNDUP(L6*F6,2)</f>
+      <c r="L6" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="10">
+    <row r="7" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" t="s" s="12">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s" s="12">
+      <c r="D7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E7" t="s" s="12">
+      <c r="E7" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>3</v>
       </c>
-      <c r="G7" t="s" s="12">
+      <c r="G7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="H7" t="s" s="12">
+      <c r="H7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I7" t="s" s="12">
+      <c r="I7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J7" t="s" s="12">
+      <c r="J7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K7" t="s" s="12">
+      <c r="K7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M7" s="15">
-        <f>ROUNDUP(L7*F7,2)</f>
+      <c r="L7" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="10">
+    <row r="8" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" t="s" s="12">
+      <c r="B8" s="10"/>
+      <c r="C8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="s" s="12">
+      <c r="D8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E8" t="s" s="12">
+      <c r="E8" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>3</v>
       </c>
-      <c r="G8" t="s" s="12">
+      <c r="G8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="H8" t="s" s="12">
+      <c r="H8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I8" t="s" s="12">
+      <c r="I8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s" s="12">
+      <c r="J8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s" s="12">
+      <c r="K8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M8" s="15">
-        <f>ROUNDUP(L8*F8,2)</f>
+      <c r="L8" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="10">
+    <row r="9" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" t="s" s="12">
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s" s="12">
+      <c r="D9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s" s="12">
+      <c r="E9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>2</v>
       </c>
-      <c r="G9" t="s" s="12">
+      <c r="G9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="H9" t="s" s="12">
+      <c r="H9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I9" t="s" s="12">
+      <c r="I9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J9" t="s" s="12">
+      <c r="J9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K9" t="s" s="12">
+      <c r="K9" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M9" s="15">
-        <f>ROUNDUP(L9*F9,2)</f>
+      <c r="L9" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="10">
+    <row r="10" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" t="s" s="12">
+      <c r="B10" s="10"/>
+      <c r="C10" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s" s="12">
+      <c r="D10" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s" s="12">
+      <c r="E10" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>4</v>
       </c>
-      <c r="G10" t="s" s="12">
+      <c r="G10" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="H10" t="s" s="12">
+      <c r="H10" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I10" t="s" s="12">
+      <c r="I10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J10" t="s" s="12">
+      <c r="J10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K10" t="s" s="12">
+      <c r="K10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="L10" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M10" s="15">
-        <f>ROUNDUP(L10*F10,2)</f>
+      <c r="L10" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="10">
+    <row r="11" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="9">
         <v>9</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" t="s" s="12">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s" s="12">
+      <c r="D11" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s" s="12">
+      <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>1</v>
       </c>
-      <c r="G11" t="s" s="12">
+      <c r="G11" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="H11" t="s" s="12">
+      <c r="H11" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I11" t="s" s="12">
+      <c r="I11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J11" t="s" s="12">
+      <c r="J11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s" s="12">
+      <c r="K11" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="L11" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M11" s="15">
-        <f>ROUNDUP(L11*F11,2)</f>
+      <c r="L11" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="10">
+    <row r="12" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" t="s" s="12">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D12" t="s" s="12">
+      <c r="D12" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s" s="12">
+      <c r="E12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <v>1</v>
       </c>
-      <c r="G12" t="s" s="12">
+      <c r="G12" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H12" t="s" s="12">
+      <c r="H12" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I12" t="s" s="12">
+      <c r="I12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J12" t="s" s="12">
+      <c r="J12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s" s="12">
+      <c r="K12" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="L12" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M12" s="15">
-        <f>ROUNDUP(L12*F12,2)</f>
+      <c r="L12" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M12" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="10">
+    <row r="13" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" t="s" s="12">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s" s="12">
+      <c r="D13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E13" t="s" s="12">
+      <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <v>1</v>
       </c>
-      <c r="G13" t="s" s="12">
+      <c r="G13" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="H13" t="s" s="12">
+      <c r="H13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I13" t="s" s="12">
+      <c r="I13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J13" t="s" s="12">
+      <c r="J13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s" s="12">
+      <c r="K13" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="L13" s="14">
-        <v>0.001</v>
-      </c>
-      <c r="M13" s="15">
-        <f>ROUNDUP(L13*F13,2)</f>
+      <c r="L13" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="M13" s="14">
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="10">
+    <row r="14" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" t="s" s="12">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D14" t="s" s="12">
+      <c r="D14" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E14" t="s" s="12">
+      <c r="E14" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <v>3</v>
       </c>
-      <c r="G14" t="s" s="12">
+      <c r="G14" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="H14" t="s" s="16">
+      <c r="H14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="I14" t="s" s="12">
+      <c r="I14" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J14" t="s" s="12">
+      <c r="J14" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K14" t="s" s="16">
+      <c r="K14" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="L14" s="14">
-        <v>0.005</v>
-      </c>
-      <c r="M14" s="15">
-        <f>ROUNDUP(L14*F14,2)</f>
+      <c r="L14" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M14" s="14">
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="10">
+    <row r="15" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" t="s" s="12">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D15" t="s" s="12">
+      <c r="D15" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E15" t="s" s="12">
+      <c r="E15" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <v>2</v>
       </c>
-      <c r="G15" t="s" s="12">
+      <c r="G15" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H15" t="s" s="12">
+      <c r="H15" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I15" t="s" s="12">
+      <c r="I15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J15" t="s" s="12">
+      <c r="J15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="K15" t="s" s="12">
+      <c r="K15" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="14">
-        <v>0.163</v>
-      </c>
-      <c r="M15" s="15">
-        <f>ROUNDUP(L15*F15,2)</f>
+      <c r="L15" s="13">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="M15" s="14">
+        <f t="shared" si="0"/>
         <v>0.33</v>
       </c>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="10">
+    <row r="16" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" t="s" s="12">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D16" t="s" s="12">
+      <c r="D16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E16" t="s" s="12">
+      <c r="E16" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <v>1</v>
       </c>
-      <c r="G16" t="s" s="12">
+      <c r="G16" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H16" t="s" s="12">
+      <c r="H16" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="I16" t="s" s="12">
+      <c r="I16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="J16" t="s" s="12">
+      <c r="J16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K16" t="s" s="12">
+      <c r="K16" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <v>0.03</v>
       </c>
-      <c r="M16" s="15">
-        <f>ROUNDUP(L16*F16,2)</f>
+      <c r="M16" s="14">
+        <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="10">
+    <row r="17" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" t="s" s="12">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s" s="12">
+      <c r="D17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="E17" t="s" s="12">
+      <c r="E17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <v>1</v>
       </c>
-      <c r="G17" t="s" s="12">
+      <c r="G17" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="H17" t="s" s="12">
+      <c r="H17" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="I17" t="s" s="12">
+      <c r="I17" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J17" t="s" s="12">
+      <c r="J17" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K17" t="s" s="12">
+      <c r="K17" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="L17" s="14">
+      <c r="L17" s="13">
         <v>2</v>
       </c>
-      <c r="M17" s="15">
-        <f>ROUNDUP(L17*F17,2)</f>
+      <c r="M17" s="14">
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="10">
+    <row r="18" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" t="s" s="12">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="D18" t="s" s="12">
+      <c r="D18" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="E18" t="s" s="12">
+      <c r="E18" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <v>1</v>
       </c>
-      <c r="G18" t="s" s="12">
+      <c r="G18" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H18" t="s" s="12">
+      <c r="H18" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I18" t="s" s="12">
+      <c r="I18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J18" t="s" s="12">
+      <c r="J18" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K18" t="s" s="12">
+      <c r="K18" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="L18" s="14">
+      <c r="L18" s="13">
         <v>0.874</v>
       </c>
-      <c r="M18" s="15">
-        <f>ROUNDUP(L18*F18,2)</f>
+      <c r="M18" s="14">
+        <f t="shared" si="0"/>
         <v>0.88</v>
       </c>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="10">
+    <row r="19" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" t="s" s="12">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="D19" t="s" s="12">
+      <c r="D19" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="E19" t="s" s="12">
+      <c r="E19" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <v>1</v>
       </c>
-      <c r="G19" t="s" s="12">
+      <c r="G19" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H19" t="s" s="12">
+      <c r="H19" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="I19" t="s" s="12">
+      <c r="I19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J19" t="s" s="12">
+      <c r="J19" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K19" t="s" s="12">
+      <c r="K19" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="14">
-        <v>0.103</v>
-      </c>
-      <c r="M19" s="15">
-        <f>ROUNDUP(L19*F19,2)</f>
+      <c r="L19" s="13">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="M19" s="14">
+        <f t="shared" si="0"/>
         <v>0.11</v>
       </c>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="10">
+    <row r="20" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" t="s" s="12">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="D20" t="s" s="12">
+      <c r="D20" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="E20" t="s" s="12">
+      <c r="E20" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <v>1</v>
       </c>
-      <c r="G20" t="s" s="12">
+      <c r="G20" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="H20" t="s" s="12">
+      <c r="H20" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="I20" t="s" s="12">
+      <c r="I20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J20" t="s" s="12">
+      <c r="J20" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="K20" t="s" s="12">
+      <c r="K20" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="L20" s="14">
-        <v>0.077</v>
-      </c>
-      <c r="M20" s="15">
-        <f>ROUNDUP(L20*F20,2)</f>
+      <c r="L20" s="13">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="M20" s="14">
+        <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="10">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s" s="17">
-        <v>107</v>
-      </c>
-      <c r="C21" t="s" s="12">
-        <v>108</v>
-      </c>
-      <c r="D21" t="s" s="12">
-        <v>109</v>
-      </c>
-      <c r="E21" t="s" s="12">
-        <v>110</v>
-      </c>
-      <c r="F21" s="13">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s" s="12">
-        <v>111</v>
-      </c>
-      <c r="H21" t="s" s="12">
-        <v>112</v>
-      </c>
-      <c r="I21" t="s" s="12">
-        <v>113</v>
-      </c>
-      <c r="J21" t="s" s="12">
-        <v>114</v>
-      </c>
-      <c r="K21" t="s" s="18">
-        <v>115</v>
-      </c>
-      <c r="L21" s="14">
-        <v>3.87</v>
-      </c>
-      <c r="M21" s="15">
-        <f>ROUNDUP(L21*F21,2)</f>
-        <v>3.87</v>
-      </c>
+    <row r="21" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="9"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="14"/>
     </row>
-    <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="10">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s" s="17">
-        <v>107</v>
-      </c>
-      <c r="C22" t="s" s="12">
-        <v>116</v>
-      </c>
-      <c r="D22" t="s" s="12">
-        <v>117</v>
-      </c>
-      <c r="E22" t="s" s="12">
-        <v>118</v>
-      </c>
-      <c r="F22" s="13">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s" s="12">
-        <v>119</v>
-      </c>
-      <c r="H22" t="s" s="12">
-        <v>120</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" t="s" s="12">
-        <v>114</v>
-      </c>
-      <c r="K22" s="19"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="15">
-        <f>ROUNDUP(L22*F22,2)</f>
-        <v>0</v>
-      </c>
+    <row r="22" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="9"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
     </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="10">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s" s="17">
-        <v>107</v>
-      </c>
-      <c r="C23" t="s" s="12">
-        <v>121</v>
-      </c>
-      <c r="D23" t="s" s="12">
-        <v>122</v>
-      </c>
-      <c r="E23" t="s" s="12">
-        <v>123</v>
-      </c>
-      <c r="F23" s="13">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s" s="12">
-        <v>121</v>
-      </c>
-      <c r="H23" t="s" s="12">
-        <v>120</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" t="s" s="12">
-        <v>114</v>
-      </c>
-      <c r="K23" s="19"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="15">
-        <f>ROUNDUP(L23*F23,2)</f>
-        <v>0</v>
-      </c>
+    <row r="23" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="9"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="26" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D26" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" location="" tooltip="" display="CL10A106MQ8NNNC"/>
-    <hyperlink ref="K3" r:id="rId2" location="" tooltip="" display="C1691"/>
-    <hyperlink ref="G4" r:id="rId3" location="" tooltip="" display="CL10A225KO8NNNC"/>
-    <hyperlink ref="K4" r:id="rId4" location="" tooltip="" display="C23630"/>
-    <hyperlink ref="G5" r:id="rId5" location="" tooltip="" display="CL10B104KB8NNNC"/>
-    <hyperlink ref="K5" r:id="rId6" location="" tooltip="" display="C1591"/>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{CD39AA46-12AE-EB44-985A-7779D8BA3506}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{E79677E6-452B-1C4E-AA8F-929E9D151E96}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{86CD2FC3-247A-AD4B-BB5B-5F3ADBD270B2}"/>
+    <hyperlink ref="K4" r:id="rId4" xr:uid="{FEC50980-0F3B-024B-8D6B-94C9998AF901}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{4373A696-C9CC-E840-9D3A-91F8FC011E78}"/>
+    <hyperlink ref="K5" r:id="rId6" xr:uid="{D1C165F6-780D-AA45-99C7-1FCEEBB46E98}"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:M8"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="16.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.33203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="9">
+        <v>19</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="12">
+        <v>1</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="13">
+        <v>3.87</v>
+      </c>
+      <c r="M3" s="14">
+        <f t="shared" ref="M3:M5" si="0">ROUNDUP(L3*F3,2)</f>
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>20</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" s="12">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" s="18"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>21</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F5" s="12">
+        <v>1</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="18"/>
+      <c r="J5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" s="18"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="D8" s="20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>